<commit_message>
Added class analysis for HPA background
Made python program to count HPA background genes in each KEGG class.
This is to use in hypergeometric test for class overrepresentation.
Commit before running code.
</commit_message>
<xml_diff>
--- a/dendogram_data_frame.xlsx
+++ b/dendogram_data_frame.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="0" windowWidth="25360" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="2840" yWindow="0" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="dendogram_data_frame.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="dendogram_data_frame.csv" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="210">
+  <si>
+    <t>cytoplasm</t>
+  </si>
+  <si>
+    <t>nucleus</t>
+  </si>
+  <si>
+    <t>nucleus/cytoplasm</t>
+  </si>
   <si>
     <t>hsa00010</t>
   </si>
@@ -640,96 +649,6 @@
   </si>
   <si>
     <t>hsa04971</t>
-  </si>
-  <si>
-    <t>hsa04972</t>
-  </si>
-  <si>
-    <t>hsa04973</t>
-  </si>
-  <si>
-    <t>hsa04974</t>
-  </si>
-  <si>
-    <t>hsa04975</t>
-  </si>
-  <si>
-    <t>hsa04976</t>
-  </si>
-  <si>
-    <t>hsa04977</t>
-  </si>
-  <si>
-    <t>hsa04978</t>
-  </si>
-  <si>
-    <t>hsa05010</t>
-  </si>
-  <si>
-    <t>hsa05012</t>
-  </si>
-  <si>
-    <t>hsa05014</t>
-  </si>
-  <si>
-    <t>hsa05016</t>
-  </si>
-  <si>
-    <t>hsa05020</t>
-  </si>
-  <si>
-    <t>hsa05030</t>
-  </si>
-  <si>
-    <t>hsa05031</t>
-  </si>
-  <si>
-    <t>hsa05032</t>
-  </si>
-  <si>
-    <t>hsa05034</t>
-  </si>
-  <si>
-    <t>hsa05100</t>
-  </si>
-  <si>
-    <t>hsa05110</t>
-  </si>
-  <si>
-    <t>hsa05120</t>
-  </si>
-  <si>
-    <t>hsa05130</t>
-  </si>
-  <si>
-    <t>hsa05131</t>
-  </si>
-  <si>
-    <t>hsa05132</t>
-  </si>
-  <si>
-    <t>hsa05133</t>
-  </si>
-  <si>
-    <t>hsa05134</t>
-  </si>
-  <si>
-    <t>hsa05140</t>
-  </si>
-  <si>
-    <t>hsa05142</t>
-  </si>
-  <si>
-    <t>pathway id</t>
-  </si>
-  <si>
-    <t>cyto_no_nuc</t>
-  </si>
-  <si>
-    <t>nuc_no_cyto</t>
-  </si>
-  <si>
-    <t>nuc_cyto_transit</t>
   </si>
 </sst>
 </file>
@@ -765,8 +684,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,107 +1018,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>233</v>
-      </c>
       <c r="B1" t="s">
-        <v>234</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>235</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>236</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>34.375</v>
+        <v>1.180994E-2</v>
       </c>
       <c r="C2">
-        <v>12.5</v>
+        <v>0.98844843000000004</v>
       </c>
       <c r="D2">
-        <v>3.125</v>
+        <v>0.79983694400000005</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>4.1666666670000003</v>
+        <v>0.95954739499999997</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>4.1666666670000003</v>
+        <v>0.65307735300000003</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>34.782608699999997</v>
+        <v>2.0831303999999998E-2</v>
       </c>
       <c r="C4">
-        <v>26.086956520000001</v>
+        <v>0.62707633900000004</v>
       </c>
       <c r="D4">
-        <v>8.6956521739999992</v>
+        <v>0.34667435899999999</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>27.272727270000001</v>
+        <v>0.47886083000000002</v>
       </c>
       <c r="D5">
-        <v>9.0909090910000003</v>
+        <v>0.26248527999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>15.78947368</v>
+        <v>0.507551211</v>
       </c>
       <c r="C6">
-        <v>42.10526316</v>
+        <v>0.111777481</v>
       </c>
       <c r="D6">
-        <v>5.263157895</v>
+        <v>0.523936332</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>28.571428569999998</v>
+        <v>0.11215863299999999</v>
       </c>
       <c r="C7">
-        <v>14.28571429</v>
+        <v>0.86913344299999995</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1206,27 +1123,27 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C8">
-        <v>33.333333330000002</v>
+        <v>0.28681956600000003</v>
       </c>
       <c r="D8">
-        <v>16.666666670000001</v>
+        <v>9.6145223000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>57.142857139999997</v>
+        <v>3.8123060000000001E-3</v>
       </c>
       <c r="C9">
-        <v>14.28571429</v>
+        <v>0.70456610799999997</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1234,13 +1151,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>7.692307692</v>
+        <v>0.89941428099999998</v>
       </c>
       <c r="C10">
-        <v>23.07692308</v>
+        <v>0.76322581700000003</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1248,10 +1165,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1262,27 +1179,27 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>22.222222219999999</v>
+        <v>0.23962407999999999</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>11.11111111</v>
+        <v>0.19301000099999999</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>5.1576373000000002E-2</v>
       </c>
       <c r="C13">
-        <v>40</v>
+        <v>0.18555782800000001</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1290,10 +1207,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>2.4040903999999998E-2</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1304,83 +1221,83 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>10.16949153</v>
+        <v>0.95178410700000005</v>
       </c>
       <c r="C15">
-        <v>13.559322030000001</v>
+        <v>0.99882626200000002</v>
       </c>
       <c r="D15">
-        <v>5.0847457629999999</v>
+        <v>0.79426370700000004</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>25</v>
+        <v>0.184673895</v>
       </c>
       <c r="C16">
-        <v>25</v>
+        <v>0.49002216900000001</v>
       </c>
       <c r="D16">
-        <v>12.5</v>
+        <v>0.159241518</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>22.549019609999998</v>
+        <v>0.15771523000000001</v>
       </c>
       <c r="C17">
-        <v>36.274509799999997</v>
+        <v>0.13263134300000001</v>
       </c>
       <c r="D17">
-        <v>10.784313729999999</v>
+        <v>0.21075101800000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>9.8591549300000008</v>
-      </c>
-      <c r="C18">
-        <v>53.521126760000001</v>
+        <v>0.97412349600000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.8800000000000001E-5</v>
       </c>
       <c r="D18">
-        <v>11.26760563</v>
+        <v>0.19043459700000001</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>45</v>
+        <v>1.8220809999999999E-3</v>
       </c>
       <c r="C19">
-        <v>10</v>
+        <v>0.97487910200000005</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>0.55219153099999996</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>33.333333330000002</v>
+        <v>3.3933455000000001E-2</v>
       </c>
       <c r="C20">
-        <v>9.5238095240000007</v>
+        <v>0.98124460499999999</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1388,27 +1305,27 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>37.037037040000001</v>
+        <v>7.8017920000000001E-3</v>
       </c>
       <c r="C21">
-        <v>25.925925929999998</v>
+        <v>0.65953565400000003</v>
       </c>
       <c r="D21">
-        <v>14.81481481</v>
+        <v>9.1583374999999995E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>10.71428571</v>
+        <v>0.81237498900000005</v>
       </c>
       <c r="C22">
-        <v>14.28571429</v>
+        <v>0.96810280000000004</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1416,10 +1333,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1430,41 +1347,41 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>2.6315789469999999</v>
+        <v>0.99694549200000004</v>
       </c>
       <c r="C24">
-        <v>31.578947370000002</v>
+        <v>0.426426939</v>
       </c>
       <c r="D24">
-        <v>7.8947368420000004</v>
+        <v>0.45538505200000001</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>20.833333329999999</v>
+        <v>0.305045228</v>
       </c>
       <c r="C25">
-        <v>16.666666670000001</v>
+        <v>0.91810218600000004</v>
       </c>
       <c r="D25">
-        <v>12.5</v>
+        <v>0.167240679</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>35.714285709999999</v>
+        <v>3.6057763E-2</v>
       </c>
       <c r="C26">
-        <v>7.1428571429999996</v>
+        <v>0.96377920800000005</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1472,52 +1389,52 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>20</v>
+        <v>0.32022287500000002</v>
       </c>
       <c r="C27">
-        <v>33.333333330000002</v>
+        <v>0.32833112199999998</v>
       </c>
       <c r="D27">
-        <v>6.6666666670000003</v>
+        <v>0.39970659200000003</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>25</v>
+        <v>0.184673895</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>0.49002216900000001</v>
       </c>
       <c r="D28">
-        <v>12.5</v>
+        <v>0.159241518</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>0.16021664899999999</v>
       </c>
       <c r="C29">
-        <v>4.1666666670000003</v>
+        <v>0.99870626100000004</v>
       </c>
       <c r="D29">
-        <v>4.1666666670000003</v>
+        <v>0.65307735300000003</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1528,27 +1445,27 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>18.75</v>
+        <v>0.36800839899999999</v>
       </c>
       <c r="C31">
-        <v>12.5</v>
+        <v>0.922756668</v>
       </c>
       <c r="D31">
-        <v>12.5</v>
+        <v>0.17148404</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32">
-        <v>25</v>
+        <v>0.37753778300000002</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1556,55 +1473,55 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>30.76923077</v>
+        <v>8.4979751000000006E-2</v>
       </c>
       <c r="C33">
-        <v>30.76923077</v>
+        <v>0.39595332700000002</v>
       </c>
       <c r="D33">
-        <v>7.692307692</v>
+        <v>0.33209106799999999</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>37.931034480000001</v>
+        <v>4.764885E-3</v>
       </c>
       <c r="C34">
-        <v>10.34482759</v>
+        <v>0.99259439699999996</v>
       </c>
       <c r="D34">
-        <v>20.689655170000002</v>
+        <v>1.2922189000000001E-2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>33.333333330000002</v>
+        <v>6.1714017000000003E-2</v>
       </c>
       <c r="C35">
-        <v>16.666666670000001</v>
+        <v>0.78494912699999997</v>
       </c>
       <c r="D35">
-        <v>8.3333333330000006</v>
+        <v>0.29742401800000001</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>0.76691027899999997</v>
       </c>
       <c r="C36">
-        <v>20</v>
+        <v>0.80874538900000004</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1612,27 +1529,27 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B37">
-        <v>20</v>
+        <v>0.29675243000000001</v>
       </c>
       <c r="C37">
-        <v>30</v>
+        <v>0.39488878799999999</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>0.227564134</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>0.59822997200000005</v>
       </c>
       <c r="C38">
-        <v>20</v>
+        <v>0.66016755299999996</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1640,38 +1557,38 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B39">
-        <v>8.3333333330000006</v>
+        <v>0.70056091200000004</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>0.55778291599999996</v>
       </c>
       <c r="D39">
-        <v>16.666666670000001</v>
+        <v>8.7791588000000004E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B40">
-        <v>21.875</v>
+        <v>0.25943304</v>
       </c>
       <c r="C40">
-        <v>18.75</v>
+        <v>0.92068673300000003</v>
       </c>
       <c r="D40">
-        <v>6.25</v>
+        <v>0.56385594900000002</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B41">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1682,13 +1599,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B42">
-        <v>40</v>
+        <v>5.1576373000000002E-2</v>
       </c>
       <c r="C42">
-        <v>40</v>
+        <v>0.18555782800000001</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1696,24 +1613,24 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B43">
-        <v>27.272727270000001</v>
+        <v>0.14277512000000001</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>27.272727270000001</v>
+        <v>1.3125443000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B44">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1724,52 +1641,52 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B45">
-        <v>20</v>
+        <v>0.24546031400000001</v>
       </c>
       <c r="C45">
-        <v>40</v>
+        <v>0.18555782800000001</v>
       </c>
       <c r="D45">
-        <v>20</v>
+        <v>6.8100308999999998E-2</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B46">
-        <v>14.28571429</v>
+        <v>0.64475083300000002</v>
       </c>
       <c r="C46">
-        <v>10.71428571</v>
+        <v>0.99018188299999998</v>
       </c>
       <c r="D46">
-        <v>3.5714285710000002</v>
+        <v>0.73499110899999998</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B47">
-        <v>30.232558139999998</v>
+        <v>2.5519152E-2</v>
       </c>
       <c r="C47">
-        <v>18.60465116</v>
+        <v>0.95801402099999999</v>
       </c>
       <c r="D47">
-        <v>9.3023255809999998</v>
+        <v>0.34927814200000001</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B48">
-        <v>33.333333330000002</v>
+        <v>7.4773527000000006E-2</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1780,24 +1697,24 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B49">
-        <v>22.222222219999999</v>
+        <v>0.23168090999999999</v>
       </c>
       <c r="C49">
-        <v>22.222222219999999</v>
+        <v>0.88760560799999999</v>
       </c>
       <c r="D49">
-        <v>4.4444444440000002</v>
+        <v>0.78724778100000004</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B50">
-        <v>23.529411759999999</v>
+        <v>0.213456799</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1808,10 +1725,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B51">
-        <v>47.058823529999998</v>
+        <v>1.8605430000000001E-3</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1822,10 +1739,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B52">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1836,13 +1753,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B53">
-        <v>50</v>
+        <v>1.4463349E-2</v>
       </c>
       <c r="C53">
-        <v>16.666666670000001</v>
+        <v>0.614876847</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1850,27 +1767,27 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B54">
-        <v>11.764705879999999</v>
+        <v>0.65928481800000005</v>
       </c>
       <c r="C54">
-        <v>5.8823529409999997</v>
+        <v>0.98631446300000003</v>
       </c>
       <c r="D54">
-        <v>11.764705879999999</v>
+        <v>0.19508953500000001</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B55">
-        <v>33.333333330000002</v>
+        <v>9.5973821000000001E-2</v>
       </c>
       <c r="C55">
-        <v>33.333333330000002</v>
+        <v>0.23711127400000001</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1878,27 +1795,27 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B56">
-        <v>20.833333329999999</v>
+        <v>0.305045228</v>
       </c>
       <c r="C56">
-        <v>4.1666666670000003</v>
+        <v>0.99870626100000004</v>
       </c>
       <c r="D56">
-        <v>4.1666666670000003</v>
+        <v>0.65307735300000003</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B57">
-        <v>23.529411759999999</v>
+        <v>0.213456799</v>
       </c>
       <c r="C57">
-        <v>5.8823529409999997</v>
+        <v>0.98631446300000003</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1906,13 +1823,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B58">
-        <v>23.529411759999999</v>
+        <v>0.213456799</v>
       </c>
       <c r="C58">
-        <v>5.8823529409999997</v>
+        <v>0.98631446300000003</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -1920,13 +1837,13 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B59">
-        <v>7.692307692</v>
+        <v>0.74304074200000003</v>
       </c>
       <c r="C59">
-        <v>7.692307692</v>
+        <v>0.95025838399999996</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1934,24 +1851,24 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60">
-        <v>36.363636360000001</v>
+        <v>4.2536174000000003E-2</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>18.18181818</v>
+        <v>7.0418977999999993E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B61">
-        <v>33.333333330000002</v>
+        <v>9.5973821000000001E-2</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1962,10 +1879,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B62">
-        <v>33.333333330000002</v>
+        <v>9.5973821000000001E-2</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1976,41 +1893,41 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B63">
-        <v>75</v>
+        <v>1.342027E-3</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>25</v>
+        <v>4.3434896000000001E-2</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B64">
-        <v>36.363636360000001</v>
+        <v>4.2536174000000003E-2</v>
       </c>
       <c r="C64">
-        <v>18.18181818</v>
+        <v>0.72815757400000003</v>
       </c>
       <c r="D64">
-        <v>9.0909090910000003</v>
+        <v>0.26248527999999999</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B65">
-        <v>20</v>
+        <v>0.24546031400000001</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>0.50552441999999997</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2018,10 +1935,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B66">
-        <v>66.666666669999998</v>
+        <v>7.0167459999999999E-3</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2032,13 +1949,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B67">
         <v>0</v>
       </c>
       <c r="C67">
-        <v>50</v>
+        <v>0.100162529</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2046,24 +1963,24 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B68">
-        <v>42.857142860000003</v>
+        <v>2.8664740000000001E-2</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>28.571428569999998</v>
+        <v>1.9616208E-2</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B69">
-        <v>20</v>
+        <v>0.29675243000000001</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2074,10 +1991,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>20</v>
+        <v>0.32022287500000002</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2088,27 +2005,27 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B71">
-        <v>36.363636360000001</v>
+        <v>4.2536174000000003E-2</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>9.0909090910000003</v>
+        <v>0.26248527999999999</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B72">
-        <v>28.571428569999998</v>
+        <v>0.133707891</v>
       </c>
       <c r="C72">
-        <v>14.28571429</v>
+        <v>0.70456610799999997</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -2116,13 +2033,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
       <c r="C73">
-        <v>25</v>
+        <v>0.49002216900000001</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2130,55 +2047,55 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74">
-        <v>48.648648649999998</v>
+        <v>75</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.0699999999999999E-5</v>
       </c>
       <c r="C74">
-        <v>5.4054054049999998</v>
+        <v>0.99987952999999996</v>
       </c>
       <c r="D74">
-        <v>13.513513509999999</v>
+        <v>0.113011511</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B75">
-        <v>25</v>
+        <v>0.176866303</v>
       </c>
       <c r="C75">
-        <v>31.25</v>
+        <v>0.39556123500000001</v>
       </c>
       <c r="D75">
-        <v>6.25</v>
+        <v>0.43230981400000001</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B76">
-        <v>26.666666670000001</v>
+        <v>0.14293106699999999</v>
       </c>
       <c r="C76">
-        <v>26.666666670000001</v>
+        <v>0.54075200000000001</v>
       </c>
       <c r="D76">
-        <v>13.33333333</v>
+        <v>0.14877675900000001</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B77">
-        <v>40</v>
+        <v>1.4223761E-2</v>
       </c>
       <c r="C77">
-        <v>40</v>
+        <v>0.164423926</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2186,13 +2103,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
       <c r="C78">
-        <v>10</v>
+        <v>0.874879352</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2200,13 +2117,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B79">
-        <v>11.11111111</v>
+        <v>0.69869139400000002</v>
       </c>
       <c r="C79">
-        <v>11.11111111</v>
+        <v>0.95550769800000002</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -2214,153 +2131,153 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B80">
-        <v>8</v>
+        <v>0.97451529299999995</v>
       </c>
       <c r="C80">
-        <v>48</v>
+        <v>5.1217520000000002E-3</v>
       </c>
       <c r="D80">
-        <v>12</v>
+        <v>0.162712938</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>79</v>
-      </c>
-      <c r="B81">
-        <v>57.31707317</v>
+        <v>82</v>
+      </c>
+      <c r="B81" s="1">
+        <v>2.7099999999999999E-15</v>
       </c>
       <c r="C81">
-        <v>9.7560975610000007</v>
+        <v>0.99999750899999995</v>
       </c>
       <c r="D81">
-        <v>1.2195121950000001</v>
+        <v>0.99629451300000005</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B82">
-        <v>28.301886790000001</v>
+        <v>7.6622440000000003E-3</v>
       </c>
       <c r="C82">
-        <v>31.13207547</v>
+        <v>0.49928770099999997</v>
       </c>
       <c r="D82">
-        <v>9.4339622639999998</v>
+        <v>0.36415165599999999</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B83">
-        <v>19.23076923</v>
+        <v>0.41082125000000003</v>
       </c>
       <c r="C83">
-        <v>44.23076923</v>
+        <v>1.9754812E-2</v>
       </c>
       <c r="D83">
-        <v>9.615384615</v>
+        <v>0.33039875099999999</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B84">
-        <v>30.35714286</v>
+        <v>1.4089849999999999E-2</v>
       </c>
       <c r="C84">
-        <v>28.571428569999998</v>
+        <v>0.63202362499999998</v>
       </c>
       <c r="D84">
-        <v>3.5714285710000002</v>
+        <v>0.89345469399999999</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B85">
         <v>0</v>
       </c>
-      <c r="C85">
-        <v>70.833333330000002</v>
+      <c r="C85" s="1">
+        <v>1.5800000000000001E-5</v>
       </c>
       <c r="D85">
-        <v>12.5</v>
+        <v>0.167240679</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B86">
-        <v>3.448275862</v>
-      </c>
-      <c r="C86">
-        <v>75.862068969999996</v>
+        <v>0.98359971499999999</v>
+      </c>
+      <c r="C86" s="1">
+        <v>1.68E-7</v>
       </c>
       <c r="D86">
-        <v>13.79310345</v>
+        <v>0.116383787</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
-      <c r="C87">
-        <v>75.862068969999996</v>
+      <c r="C87" s="1">
+        <v>1.68E-7</v>
       </c>
       <c r="D87">
-        <v>10.34482759</v>
+        <v>0.26542734499999998</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B88">
-        <v>2.0833333330000001</v>
-      </c>
-      <c r="C88">
-        <v>79.166666669999998</v>
+        <v>0.99999965400000002</v>
+      </c>
+      <c r="C88" s="1">
+        <v>8.7500000000000001E-23</v>
       </c>
       <c r="D88">
-        <v>7.2916666670000003</v>
+        <v>0.65037310199999998</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B89">
-        <v>17.14285714</v>
+        <v>0.51708726000000005</v>
       </c>
       <c r="C89">
-        <v>25.714285709999999</v>
+        <v>0.71175752299999995</v>
       </c>
       <c r="D89">
-        <v>20</v>
+        <v>1.131208E-2</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B90">
-        <v>35.714285709999999</v>
+        <v>3.6057763E-2</v>
       </c>
       <c r="C90">
-        <v>21.428571430000002</v>
+        <v>0.69361203100000002</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2368,83 +2285,83 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B91">
-        <v>12.90322581</v>
+        <v>0.73512101900000004</v>
       </c>
       <c r="C91">
-        <v>16.129032259999999</v>
+        <v>0.95792154900000004</v>
       </c>
       <c r="D91">
-        <v>9.6774193549999996</v>
+        <v>0.307362845</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B92">
-        <v>8</v>
-      </c>
-      <c r="C92">
-        <v>76</v>
+        <v>0.88356983899999997</v>
+      </c>
+      <c r="C92" s="1">
+        <v>8.7199999999999997E-7</v>
       </c>
       <c r="D92">
-        <v>8</v>
+        <v>0.39774152200000001</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B93">
-        <v>3.125</v>
-      </c>
-      <c r="C93">
-        <v>81.25</v>
+        <v>0.99057032499999997</v>
+      </c>
+      <c r="C93" s="1">
+        <v>9.859999999999999E-10</v>
       </c>
       <c r="D93">
-        <v>6.25</v>
+        <v>0.56385594900000002</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>0</v>
       </c>
-      <c r="C94">
-        <v>89.473684210000002</v>
+      <c r="C94" s="1">
+        <v>1.31E-8</v>
       </c>
       <c r="D94">
-        <v>5.263157895</v>
+        <v>0.523936332</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>0</v>
       </c>
       <c r="C95">
-        <v>55.555555560000002</v>
+        <v>9.4187990000000003E-3</v>
       </c>
       <c r="D95">
-        <v>11.11111111</v>
+        <v>0.21942400100000001</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B96">
         <v>0</v>
       </c>
-      <c r="C96">
-        <v>90</v>
+      <c r="C96" s="1">
+        <v>9.9799999999999993E-6</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2452,349 +2369,349 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B97">
-        <v>10</v>
+        <v>0.904627195</v>
       </c>
       <c r="C97">
-        <v>50</v>
+        <v>4.8511090000000002E-3</v>
       </c>
       <c r="D97">
-        <v>7.5</v>
+        <v>0.49610717799999998</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B98">
-        <v>19.6969697</v>
+        <v>0.38526790900000002</v>
       </c>
       <c r="C98">
-        <v>32.575757580000001</v>
+        <v>0.36920728400000002</v>
       </c>
       <c r="D98">
-        <v>14.39393939</v>
+        <v>1.4965899E-2</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B99">
-        <v>28</v>
+        <v>4.3306567999999997E-2</v>
       </c>
       <c r="C99">
-        <v>26</v>
+        <v>0.757842872</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>0.94855309899999996</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B100">
-        <v>26.666666670000001</v>
+        <v>2.9183437999999999E-2</v>
       </c>
       <c r="C100">
-        <v>24.444444440000002</v>
+        <v>0.915867824</v>
       </c>
       <c r="D100">
-        <v>6.6666666670000003</v>
+        <v>0.71803172599999998</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B101">
-        <v>25.80645161</v>
+        <v>4.2302126000000002E-2</v>
       </c>
       <c r="C101">
-        <v>24.731182799999999</v>
+        <v>0.91033855299999999</v>
       </c>
       <c r="D101">
-        <v>6.451612903</v>
+        <v>0.749414307</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B102">
-        <v>20.33898305</v>
+        <v>0.33502605200000002</v>
       </c>
       <c r="C102">
-        <v>18.644067799999998</v>
+        <v>0.98143319200000001</v>
       </c>
       <c r="D102">
-        <v>3.3898305080000002</v>
+        <v>0.91265183699999997</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B103">
-        <v>26.666666670000001</v>
+        <v>3.9762960999999999E-2</v>
       </c>
       <c r="C103">
-        <v>28</v>
+        <v>0.70795528799999996</v>
       </c>
       <c r="D103">
-        <v>9.3333333330000006</v>
+        <v>0.36857854899999998</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B104">
-        <v>27.941176469999998</v>
+        <v>2.6873439999999998E-2</v>
       </c>
       <c r="C104">
-        <v>30.882352940000001</v>
+        <v>0.49612726699999998</v>
       </c>
       <c r="D104">
-        <v>1.4705882349999999</v>
+        <v>0.98800953300000005</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B105">
-        <v>36.231884059999999</v>
+        <v>2.4340599999999999E-4</v>
       </c>
       <c r="C105">
-        <v>24.63768116</v>
+        <v>0.87139781999999999</v>
       </c>
       <c r="D105">
-        <v>8.6956521739999992</v>
+        <v>0.43555768</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B106">
-        <v>23.809523810000002</v>
+        <v>0.13597562699999999</v>
       </c>
       <c r="C106">
-        <v>26.984126979999999</v>
+        <v>0.74337217700000002</v>
       </c>
       <c r="D106">
-        <v>3.1746031750000001</v>
+        <v>0.93335748900000004</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B107">
-        <v>27.777777780000001</v>
+        <v>4.1948302999999999E-2</v>
       </c>
       <c r="C107">
-        <v>22.222222219999999</v>
+        <v>0.91399334700000001</v>
       </c>
       <c r="D107">
-        <v>12.96296296</v>
+        <v>0.11138118700000001</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B108">
-        <v>32.142857139999997</v>
+        <v>6.2873319999999996E-3</v>
       </c>
       <c r="C108">
-        <v>23.214285709999999</v>
+        <v>0.89032047000000003</v>
       </c>
       <c r="D108">
-        <v>5.3571428570000004</v>
+        <v>0.759134635</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B109">
-        <v>16.883116879999999</v>
+        <v>0.63184742500000002</v>
       </c>
       <c r="C109">
-        <v>32.467532470000002</v>
+        <v>0.38554915200000001</v>
       </c>
       <c r="D109">
-        <v>10.38961039</v>
+        <v>0.26023054699999998</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B110">
-        <v>29.09090909</v>
+        <v>2.4726714E-2</v>
       </c>
       <c r="C110">
-        <v>20</v>
+        <v>0.96103199100000003</v>
       </c>
       <c r="D110">
-        <v>3.636363636</v>
+        <v>0.886258977</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B111">
-        <v>30.90909091</v>
+        <v>1.1581898E-2</v>
       </c>
       <c r="C111">
-        <v>18.18181818</v>
+        <v>0.98128935500000003</v>
       </c>
       <c r="D111">
-        <v>3.636363636</v>
+        <v>0.886258977</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B112">
-        <v>29.166666670000001</v>
+        <v>7.2089202000000005E-2</v>
       </c>
       <c r="C112">
-        <v>12.5</v>
+        <v>0.97075484999999995</v>
       </c>
       <c r="D112">
-        <v>4.1666666670000003</v>
+        <v>0.65307735300000003</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B113">
-        <v>8.8235294119999992</v>
-      </c>
-      <c r="C113">
-        <v>55.882352939999997</v>
+        <v>0.99683876400000004</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1.1000000000000001E-7</v>
       </c>
       <c r="D113">
-        <v>17.647058820000002</v>
+        <v>1.798064E-3</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B114">
-        <v>20.3125</v>
+        <v>0.33624538599999998</v>
       </c>
       <c r="C114">
-        <v>35.9375</v>
+        <v>0.189851503</v>
       </c>
       <c r="D114">
-        <v>10.9375</v>
+        <v>0.21998573599999999</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B115">
-        <v>20.408163269999999</v>
+        <v>0.331310985</v>
       </c>
       <c r="C115">
-        <v>34.693877550000003</v>
+        <v>0.26626158700000002</v>
       </c>
       <c r="D115">
-        <v>18.367346940000001</v>
+        <v>1.1114862E-2</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B116">
-        <v>21.348314609999999</v>
+        <v>0.24847186299999999</v>
       </c>
       <c r="C116">
-        <v>38.202247190000001</v>
+        <v>7.5342813999999994E-2</v>
       </c>
       <c r="D116">
-        <v>11.23595506</v>
+        <v>0.17958985799999999</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B117">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C117">
         <v>0</v>
       </c>
       <c r="D117">
-        <v>16.666666670000001</v>
+        <v>9.6145223000000002E-2</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B118">
-        <v>10.52631579</v>
+        <v>0.73453017799999998</v>
       </c>
       <c r="C118">
-        <v>5.263157895</v>
+        <v>0.99295036400000003</v>
       </c>
       <c r="D118">
-        <v>10.52631579</v>
+        <v>0.24432521200000001</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B119">
-        <v>16.666666670000001</v>
+        <v>0.41155667200000001</v>
       </c>
       <c r="C119">
-        <v>16.666666670000001</v>
+        <v>0.78494912699999997</v>
       </c>
       <c r="D119">
-        <v>25</v>
+        <v>1.8301147E-2</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B120">
-        <v>25.773195879999999</v>
+        <v>4.0252191999999999E-2</v>
       </c>
       <c r="C120">
-        <v>14.432989689999999</v>
+        <v>0.99992315099999995</v>
       </c>
       <c r="D120">
-        <v>5.1546391749999998</v>
+        <v>0.88369624300000005</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B121">
-        <v>31.481481479999999</v>
+        <v>9.4408849999999996E-3</v>
       </c>
       <c r="C121">
-        <v>9.2592592590000002</v>
+        <v>0.99990311799999998</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -2802,111 +2719,111 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B122">
-        <v>25.65789474</v>
+        <v>1.8043311999999999E-2</v>
       </c>
       <c r="C122">
-        <v>11.84210526</v>
+        <v>0.999999992</v>
       </c>
       <c r="D122">
-        <v>5.9210526320000003</v>
+        <v>0.89250133300000001</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B123">
-        <v>20</v>
+        <v>0.35757409099999998</v>
       </c>
       <c r="C123">
-        <v>18</v>
+        <v>0.97708321300000001</v>
       </c>
       <c r="D123">
-        <v>4</v>
+        <v>0.843413839</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B124">
-        <v>13.636363640000001</v>
+        <v>0.76474150100000005</v>
       </c>
       <c r="C124">
-        <v>15.90909091</v>
+        <v>0.98546277000000004</v>
       </c>
       <c r="D124">
-        <v>2.2727272730000001</v>
+        <v>0.91795021799999998</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B125">
-        <v>39.024390240000002</v>
+        <v>8.0810699999999997E-4</v>
       </c>
       <c r="C125">
-        <v>21.951219510000001</v>
+        <v>0.88100408399999997</v>
       </c>
       <c r="D125">
-        <v>9.7560975610000007</v>
+        <v>0.31230110700000002</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B126">
-        <v>29.487179489999999</v>
+        <v>5.9485199999999999E-4</v>
       </c>
       <c r="C126">
-        <v>26.92307692</v>
+        <v>0.88485002800000001</v>
       </c>
       <c r="D126">
-        <v>7.692307692</v>
+        <v>0.665737841</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B127">
-        <v>35.9375</v>
+        <v>4.5295300000000003E-4</v>
       </c>
       <c r="C127">
-        <v>20.3125</v>
+        <v>0.96934589699999996</v>
       </c>
       <c r="D127">
-        <v>12.5</v>
+        <v>0.121447837</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B128">
-        <v>27.906976740000001</v>
+        <v>5.4372365999999998E-2</v>
       </c>
       <c r="C128">
-        <v>9.3023255809999998</v>
+        <v>0.99945693999999996</v>
       </c>
       <c r="D128">
-        <v>11.627906980000001</v>
+        <v>0.18985540300000001</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B129">
-        <v>4.7619047620000003</v>
+        <v>0.93148952100000004</v>
       </c>
       <c r="C129">
-        <v>23.809523810000002</v>
+        <v>0.69701001600000001</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -2914,13 +2831,13 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B130">
-        <v>21.15384615</v>
+        <v>0.28459889599999999</v>
       </c>
       <c r="C130">
-        <v>36.53846154</v>
+        <v>0.18073520700000001</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -2928,55 +2845,55 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B131">
-        <v>34.090909089999997</v>
+        <v>5.5391340000000002E-3</v>
       </c>
       <c r="C131">
-        <v>29.545454549999999</v>
+        <v>0.54732828099999997</v>
       </c>
       <c r="D131">
-        <v>4.5454545450000001</v>
+        <v>0.77419571099999995</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B132">
-        <v>10.958904110000001</v>
+        <v>0.95570941099999995</v>
       </c>
       <c r="C132">
-        <v>38.356164380000003</v>
+        <v>8.8161082000000002E-2</v>
       </c>
       <c r="D132">
-        <v>10.958904110000001</v>
+        <v>0.212760538</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B133">
-        <v>14.28571429</v>
+        <v>0.51982461000000002</v>
       </c>
       <c r="C133">
-        <v>50</v>
+        <v>4.2858229999999997E-2</v>
       </c>
       <c r="D133">
-        <v>7.1428571429999996</v>
+        <v>0.36624928099999998</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B134">
-        <v>10.71428571</v>
+        <v>0.81237498900000005</v>
       </c>
       <c r="C134">
-        <v>60.714285709999999</v>
+        <v>3.7932500000000002E-4</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -2984,13 +2901,13 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B135">
-        <v>15</v>
+        <v>0.55104294099999995</v>
       </c>
       <c r="C135">
-        <v>40</v>
+        <v>0.14840628</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -2998,209 +2915,209 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B136">
-        <v>17.391304349999999</v>
+        <v>0.53109583500000002</v>
       </c>
       <c r="C136">
-        <v>40.816326529999998</v>
+        <v>6.4632762999999996E-2</v>
       </c>
       <c r="D136">
-        <v>12.244897959999999</v>
+        <v>0.15092198700000001</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B137">
-        <v>22</v>
+        <v>0.23819633700000001</v>
       </c>
       <c r="C137">
-        <v>26</v>
+        <v>0.757842872</v>
       </c>
       <c r="D137">
-        <v>12</v>
+        <v>0.162712938</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B138">
-        <v>32.352941180000002</v>
+        <v>1.9751149999999999E-2</v>
       </c>
       <c r="C138">
-        <v>23.529411759999999</v>
+        <v>0.79618952399999998</v>
       </c>
       <c r="D138">
-        <v>2.9411764709999999</v>
+        <v>0.82666332200000003</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B139">
-        <v>26.229508200000001</v>
+        <v>6.2544155000000004E-2</v>
       </c>
       <c r="C139">
-        <v>31.147540979999999</v>
+        <v>0.47220898500000003</v>
       </c>
       <c r="D139">
-        <v>9.8360655739999991</v>
+        <v>0.313728854</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B140">
-        <v>18.07228916</v>
+        <v>0.53310264200000002</v>
       </c>
       <c r="C140">
-        <v>27.710843369999999</v>
+        <v>0.74170579199999997</v>
       </c>
       <c r="D140">
-        <v>6.0240963860000001</v>
+        <v>0.77464972899999995</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B141">
-        <v>27.826086960000001</v>
+        <v>8.2571429999999998E-3</v>
       </c>
       <c r="C141">
-        <v>20.869565219999998</v>
+        <v>0.99332665399999998</v>
       </c>
       <c r="D141">
-        <v>4.3478260869999996</v>
+        <v>0.95556838600000005</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B142">
-        <v>29.545454549999999</v>
+        <v>3.1029844000000001E-2</v>
       </c>
       <c r="C142">
-        <v>13.636363640000001</v>
+        <v>0.99471642100000002</v>
       </c>
       <c r="D142">
-        <v>6.8181818180000002</v>
+        <v>0.57324464500000005</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B143">
-        <v>14.58333333</v>
+        <v>0.725298636</v>
       </c>
       <c r="C143">
-        <v>18.75</v>
+        <v>0.96600910100000004</v>
       </c>
       <c r="D143">
-        <v>4.1666666670000003</v>
+        <v>0.82268875799999996</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B144">
-        <v>11.32075472</v>
+        <v>0.90461891000000005</v>
       </c>
       <c r="C144">
-        <v>32.075471700000001</v>
+        <v>0.40850434499999999</v>
       </c>
       <c r="D144">
-        <v>5.6603773579999999</v>
+        <v>0.71953185900000005</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B145">
-        <v>22.388059699999999</v>
+        <v>0.20006691400000001</v>
       </c>
       <c r="C145">
-        <v>22.388059699999999</v>
+        <v>0.93693721699999999</v>
       </c>
       <c r="D145">
-        <v>4.4776119400000001</v>
+        <v>0.86804278800000001</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B146">
-        <v>23.529411759999999</v>
+        <v>0.189355888</v>
       </c>
       <c r="C146">
-        <v>32.352941180000002</v>
+        <v>0.38474335100000001</v>
       </c>
       <c r="D146">
-        <v>5.8823529409999997</v>
+        <v>0.60596596899999999</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B147">
-        <v>11.53846154</v>
+        <v>0.94811946999999996</v>
       </c>
       <c r="C147">
-        <v>41.025641030000003</v>
+        <v>3.0140644000000001E-2</v>
       </c>
       <c r="D147">
-        <v>5.1282051280000003</v>
+        <v>0.84668154299999998</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B148">
-        <v>23.809523810000002</v>
+        <v>0.200312672</v>
       </c>
       <c r="C148">
-        <v>9.5238095240000007</v>
+        <v>0.98124460499999999</v>
       </c>
       <c r="D148">
-        <v>4.7619047620000003</v>
+        <v>0.57924084600000003</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B149">
-        <v>28.07017544</v>
+        <v>3.4615883E-2</v>
       </c>
       <c r="C149">
-        <v>22.80701754</v>
+        <v>0.905269035</v>
       </c>
       <c r="D149">
-        <v>3.50877193</v>
+        <v>0.90023931599999996</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B150">
-        <v>16.666666670000001</v>
+        <v>0.49817434399999999</v>
       </c>
       <c r="C150">
-        <v>25</v>
+        <v>0.676937962</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -3208,13 +3125,13 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B151">
-        <v>40</v>
+        <v>5.1576373000000002E-2</v>
       </c>
       <c r="C151">
-        <v>20</v>
+        <v>0.50552441999999997</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -3222,279 +3139,279 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B152">
-        <v>30.434782609999999</v>
+        <v>2.0900351000000001E-2</v>
       </c>
       <c r="C152">
-        <v>23.913043479999999</v>
+        <v>0.83441761999999997</v>
       </c>
       <c r="D152">
-        <v>10.86956522</v>
+        <v>0.234213264</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B153">
-        <v>25.80645161</v>
+        <v>0.12292311</v>
       </c>
       <c r="C153">
-        <v>9.6774193549999996</v>
+        <v>0.99582613600000003</v>
       </c>
       <c r="D153">
-        <v>16.129032259999999</v>
+        <v>5.6310780999999997E-2</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B154">
-        <v>33.333333330000002</v>
+        <v>1.5397289E-2</v>
       </c>
       <c r="C154">
-        <v>15.15151515</v>
+        <v>0.97346981499999996</v>
       </c>
       <c r="D154">
-        <v>12.121212119999999</v>
+        <v>0.174132919</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B155">
-        <v>23.333333329999999</v>
+        <v>0.202699619</v>
       </c>
       <c r="C155">
-        <v>43.333333330000002</v>
+        <v>6.0759541E-2</v>
       </c>
       <c r="D155">
-        <v>13.33333333</v>
+        <v>0.129858583</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B156">
-        <v>31.343283580000001</v>
+        <v>5.3501859999999998E-3</v>
       </c>
       <c r="C156">
-        <v>23.880597009999999</v>
+        <v>0.89463193299999999</v>
       </c>
       <c r="D156">
-        <v>7.4626865670000004</v>
+        <v>0.57388882399999996</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B157">
-        <v>18.18181818</v>
+        <v>0.41683019199999999</v>
       </c>
       <c r="C157">
-        <v>18.18181818</v>
+        <v>0.87313502799999998</v>
       </c>
       <c r="D157">
-        <v>9.0909090910000003</v>
+        <v>0.32094221299999998</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B158">
-        <v>34.090909089999997</v>
+        <v>5.5391340000000002E-3</v>
       </c>
       <c r="C158">
-        <v>29.545454549999999</v>
+        <v>0.54732828099999997</v>
       </c>
       <c r="D158">
-        <v>6.8181818180000002</v>
+        <v>0.57324464500000005</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B159">
-        <v>27.777777780000001</v>
+        <v>4.1948302999999999E-2</v>
       </c>
       <c r="C159">
-        <v>31.481481479999999</v>
+        <v>0.445484239</v>
       </c>
       <c r="D159">
-        <v>7.407407407</v>
+        <v>0.54817114600000005</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B160">
-        <v>26.315789469999999</v>
+        <v>9.5602102999999994E-2</v>
       </c>
       <c r="C160">
-        <v>31.578947370000002</v>
+        <v>0.426426939</v>
       </c>
       <c r="D160">
-        <v>10.52631579</v>
+        <v>0.25804497300000001</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B161">
-        <v>31.25</v>
+        <v>3.0593939000000001E-2</v>
       </c>
       <c r="C161">
-        <v>34.375</v>
+        <v>0.29523238699999999</v>
       </c>
       <c r="D161">
-        <v>3.125</v>
+        <v>0.79983694400000005</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B162">
-        <v>38.46153846</v>
+        <v>3.1508099999999999E-4</v>
       </c>
       <c r="C162">
-        <v>19.23076923</v>
+        <v>0.96665796699999995</v>
       </c>
       <c r="D162">
-        <v>5.769230769</v>
+        <v>0.70530961400000003</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B163">
-        <v>26.865671639999999</v>
+        <v>4.3378888999999997E-2</v>
       </c>
       <c r="C163">
-        <v>29.850746269999998</v>
+        <v>0.56777623300000002</v>
       </c>
       <c r="D163">
-        <v>13.432835819999999</v>
+        <v>7.7981352000000004E-2</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B164">
-        <v>21.276595740000001</v>
+        <v>0.280155125</v>
       </c>
       <c r="C164">
-        <v>12.76595745</v>
+        <v>0.99751628699999995</v>
       </c>
       <c r="D164">
-        <v>2.1276595739999999</v>
+        <v>0.93493581800000003</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B165">
-        <v>25</v>
+        <v>0.184673895</v>
       </c>
       <c r="C165">
-        <v>12.5</v>
+        <v>0.77608075399999998</v>
       </c>
       <c r="D165">
-        <v>37.5</v>
+        <v>3.4719550000000001E-3</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B166">
-        <v>10</v>
+        <v>0.76691027899999997</v>
       </c>
       <c r="C166">
-        <v>50</v>
+        <v>2.5609124E-2</v>
       </c>
       <c r="D166">
-        <v>30</v>
+        <v>1.3161049999999999E-3</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B167">
-        <v>25</v>
+        <v>0.15171905699999999</v>
       </c>
       <c r="C167">
-        <v>39.285714290000001</v>
+        <v>0.14206142199999999</v>
       </c>
       <c r="D167">
-        <v>7.1428571429999996</v>
+        <v>0.47199477099999998</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B168">
-        <v>22.222222219999999</v>
+        <v>0.24843362899999999</v>
       </c>
       <c r="C168">
-        <v>40.74074074</v>
+        <v>0.112183303</v>
       </c>
       <c r="D168">
-        <v>3.703703704</v>
+        <v>0.71620565599999997</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B169">
-        <v>23.07692308</v>
+        <v>0.21742704400000001</v>
       </c>
       <c r="C169">
-        <v>11.53846154</v>
+        <v>0.98292248900000001</v>
       </c>
       <c r="D169">
-        <v>15.38461538</v>
+        <v>8.0317549000000002E-2</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B170">
-        <v>29.113924050000001</v>
+        <v>1.0854878E-2</v>
       </c>
       <c r="C170">
-        <v>35.443037969999999</v>
+        <v>0.1967778</v>
       </c>
       <c r="D170">
-        <v>8.8607594939999998</v>
+        <v>0.42538039100000002</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B171">
-        <v>19.047619050000002</v>
+        <v>0.37523167299999999</v>
       </c>
       <c r="C171">
-        <v>38.095238100000003</v>
+        <v>0.190149816</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -3502,27 +3419,27 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B172">
-        <v>21.212121209999999</v>
+        <v>0.28943566399999998</v>
       </c>
       <c r="C172">
-        <v>27.272727270000001</v>
+        <v>0.63050939900000003</v>
       </c>
       <c r="D172">
-        <v>3.0303030299999998</v>
+        <v>0.81368112500000001</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B173">
-        <v>24.242424239999998</v>
+        <v>0.16567483899999999</v>
       </c>
       <c r="C173">
-        <v>42.424242419999999</v>
+        <v>6.7072862999999996E-2</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -3530,13 +3447,13 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B174">
-        <v>30.76923077</v>
+        <v>4.6340872999999998E-2</v>
       </c>
       <c r="C174">
-        <v>30.76923077</v>
+        <v>0.44450611000000001</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -3544,13 +3461,13 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B175">
-        <v>31.25</v>
+        <v>6.8273547000000004E-2</v>
       </c>
       <c r="C175">
-        <v>18.75</v>
+        <v>0.79668072899999998</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -3558,27 +3475,27 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B176">
-        <v>18.75</v>
+        <v>0.44048515599999999</v>
       </c>
       <c r="C176">
-        <v>33.333333330000002</v>
+        <v>0.33655297000000001</v>
       </c>
       <c r="D176">
-        <v>2.0833333330000001</v>
+        <v>0.939816125</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B177">
-        <v>40</v>
+        <v>7.3999599999999997E-3</v>
       </c>
       <c r="C177">
-        <v>25</v>
+        <v>0.64522792399999995</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -3586,13 +3503,13 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B178">
-        <v>20</v>
+        <v>0.29675243000000001</v>
       </c>
       <c r="C178">
-        <v>40</v>
+        <v>0.17991346999999999</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -3600,13 +3517,13 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B179">
-        <v>20</v>
+        <v>0.24546031400000001</v>
       </c>
       <c r="C179">
-        <v>60</v>
+        <v>3.7436055000000003E-2</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -3614,13 +3531,13 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B180">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C180">
-        <v>33.333333330000002</v>
+        <v>0.28681956600000003</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -3628,55 +3545,55 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B181">
-        <v>32.352941180000002</v>
+        <v>1.9751149999999999E-2</v>
       </c>
       <c r="C181">
-        <v>20.58823529</v>
+        <v>0.88843289800000003</v>
       </c>
       <c r="D181">
-        <v>2.9411764709999999</v>
+        <v>0.82666332200000003</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B182">
-        <v>29.52380952</v>
+        <v>3.4360440000000001E-3</v>
       </c>
       <c r="C182">
-        <v>17.14285714</v>
+        <v>0.99944712000000002</v>
       </c>
       <c r="D182">
-        <v>2.8571428569999999</v>
+        <v>0.98860076799999996</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
-        <v>181</v>
-      </c>
-      <c r="B183">
-        <v>40.78947368</v>
+        <v>184</v>
+      </c>
+      <c r="B183" s="1">
+        <v>3.2499999999999998E-6</v>
       </c>
       <c r="C183">
-        <v>19.736842110000001</v>
+        <v>0.98562554300000005</v>
       </c>
       <c r="D183">
-        <v>6.5789473679999997</v>
+        <v>0.69700373999999998</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B184">
-        <v>25</v>
+        <v>0.15171905699999999</v>
       </c>
       <c r="C184">
-        <v>50</v>
+        <v>1.3047815000000001E-2</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -3684,27 +3601,27 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B185">
-        <v>22.727272729999999</v>
+        <v>0.20875396199999999</v>
       </c>
       <c r="C185">
-        <v>36.363636360000001</v>
+        <v>0.199932525</v>
       </c>
       <c r="D185">
-        <v>4.5454545450000001</v>
+        <v>0.77419571099999995</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B186">
-        <v>18.18181818</v>
+        <v>0.35449392200000002</v>
       </c>
       <c r="C186">
-        <v>27.272727270000001</v>
+        <v>0.47886083000000002</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -3712,27 +3629,27 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B187">
-        <v>18.75</v>
+        <v>0.44048515599999999</v>
       </c>
       <c r="C187">
-        <v>39.583333330000002</v>
+        <v>9.2037848000000005E-2</v>
       </c>
       <c r="D187">
-        <v>8.3333333330000006</v>
+        <v>0.44191972099999999</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B188">
-        <v>26.41509434</v>
+        <v>6.8663667999999997E-2</v>
       </c>
       <c r="C188">
-        <v>41.509433960000003</v>
+        <v>4.7533964999999997E-2</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -3740,13 +3657,13 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B189">
-        <v>21.951219510000001</v>
+        <v>0.248842376</v>
       </c>
       <c r="C189">
-        <v>41.463414630000003</v>
+        <v>6.6635403999999995E-2</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -3754,27 +3671,27 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B190">
-        <v>28.205128210000002</v>
+        <v>5.588576E-2</v>
       </c>
       <c r="C190">
-        <v>35.897435899999998</v>
+        <v>0.225813442</v>
       </c>
       <c r="D190">
-        <v>5.1282051280000003</v>
+        <v>0.69889955500000001</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B191">
-        <v>32.258064519999998</v>
+        <v>2.4136939E-2</v>
       </c>
       <c r="C191">
-        <v>38.709677419999998</v>
+        <v>0.149413095</v>
       </c>
       <c r="D191">
         <v>0</v>
@@ -3782,136 +3699,136 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B192">
-        <v>23.880597009999999</v>
+        <v>0.12799460800000001</v>
       </c>
       <c r="C192">
-        <v>38.80597015</v>
+        <v>8.3296134999999993E-2</v>
       </c>
       <c r="D192">
-        <v>4.4776119400000001</v>
+        <v>0.86804278800000001</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B193">
-        <v>31.428571430000002</v>
+        <v>2.4958581000000001E-2</v>
       </c>
       <c r="C193">
-        <v>17.14285714</v>
+        <v>0.957401787</v>
       </c>
       <c r="D193">
-        <v>14.28571429</v>
+        <v>9.1693585999999994E-2</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B194">
-        <v>30.3030303</v>
+        <v>9.5295499999999995E-3</v>
       </c>
       <c r="C194">
-        <v>25.757575760000002</v>
+        <v>0.81529458399999999</v>
       </c>
       <c r="D194">
-        <v>7.575757576</v>
+        <v>0.55876459700000003</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B195">
-        <v>29.166666670000001</v>
+        <v>3.0623648999999999E-2</v>
       </c>
       <c r="C195">
-        <v>33.333333330000002</v>
+        <v>0.33655297000000001</v>
       </c>
       <c r="D195">
-        <v>8.3333333330000006</v>
+        <v>0.44191972099999999</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B196">
-        <v>26.086956520000001</v>
+        <v>0.13451281100000001</v>
       </c>
       <c r="C196">
-        <v>26.086956520000001</v>
+        <v>0.62707633900000004</v>
       </c>
       <c r="D196">
-        <v>4.3478260869999996</v>
+        <v>0.62967988500000005</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B197">
-        <v>15</v>
+        <v>0.55104294099999995</v>
       </c>
       <c r="C197">
-        <v>30</v>
+        <v>0.45581036699999999</v>
       </c>
       <c r="D197">
-        <v>5</v>
+        <v>0.55219153099999996</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B198">
-        <v>41.176470590000001</v>
+        <v>8.3176299999999995E-3</v>
       </c>
       <c r="C198">
-        <v>23.529411759999999</v>
+        <v>0.66688924000000005</v>
       </c>
       <c r="D198">
-        <v>11.764705879999999</v>
+        <v>0.19508953500000001</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B199">
         <v>0</v>
       </c>
       <c r="C199">
-        <v>22.950819670000001</v>
+        <v>0.91048873900000005</v>
       </c>
       <c r="D199">
-        <v>11.475409839999999</v>
+        <v>0.183896693</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B200">
-        <v>17.647058820000002</v>
+        <v>0.552150001</v>
       </c>
       <c r="C200">
-        <v>17.647058820000002</v>
+        <v>0.99306377499999998</v>
       </c>
       <c r="D200">
-        <v>10.29411765</v>
+        <v>0.27170122899999999</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B201">
-        <v>37.5</v>
+        <v>4.8764551000000003E-2</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -3922,13 +3839,13 @@
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B202">
-        <v>16.666666670000001</v>
+        <v>0.32384577199999998</v>
       </c>
       <c r="C202">
-        <v>83.333333330000002</v>
+        <v>1.0019079999999999E-3</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -3936,27 +3853,27 @@
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B203">
-        <v>33.333333330000002</v>
+        <v>6.1714017000000003E-2</v>
       </c>
       <c r="C203">
-        <v>25</v>
+        <v>0.55778291599999996</v>
       </c>
       <c r="D203">
-        <v>16.666666670000001</v>
+        <v>8.7791588000000004E-2</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B204">
-        <v>26.315789469999999</v>
+        <v>0.139509045</v>
       </c>
       <c r="C204">
-        <v>21.05263158</v>
+        <v>0.76786602299999995</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -3964,13 +3881,13 @@
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B205">
-        <v>40</v>
+        <v>3.875159E-3</v>
       </c>
       <c r="C205">
-        <v>28</v>
+        <v>0.560106561</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -3978,422 +3895,79 @@
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B206">
-        <v>18.18181818</v>
+        <v>0.35449392200000002</v>
       </c>
       <c r="C206">
-        <v>27.272727270000001</v>
+        <v>0.47886083000000002</v>
       </c>
       <c r="D206">
-        <v>18.18181818</v>
+        <v>7.0418977999999993E-2</v>
       </c>
     </row>
     <row r="207" spans="1:4">
       <c r="A207" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B207">
-        <v>22.727272729999999</v>
+        <v>0.23379670799999999</v>
       </c>
       <c r="C207">
-        <v>22.727272729999999</v>
+        <v>0.74345675499999997</v>
       </c>
       <c r="D207">
-        <v>4.5454545450000001</v>
+        <v>0.60507070900000004</v>
       </c>
     </row>
     <row r="208" spans="1:4">
       <c r="A208" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B208">
-        <v>27.777777780000001</v>
+        <v>0.11285305700000001</v>
       </c>
       <c r="C208">
-        <v>22.222222219999999</v>
+        <v>0.72063882099999998</v>
       </c>
       <c r="D208">
-        <v>5.5555555559999998</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4">
-      <c r="A209" t="s">
-        <v>207</v>
-      </c>
-      <c r="B209">
-        <v>17.85714286</v>
-      </c>
-      <c r="C209">
-        <v>17.85714286</v>
-      </c>
-      <c r="D209">
-        <v>3.5714285710000002</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4">
-      <c r="A210" t="s">
-        <v>208</v>
-      </c>
-      <c r="B210">
-        <v>42.857142860000003</v>
-      </c>
-      <c r="C210">
-        <v>14.28571429</v>
-      </c>
-      <c r="D210">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4">
-      <c r="A211" t="s">
-        <v>209</v>
-      </c>
-      <c r="B211">
-        <v>12.5</v>
-      </c>
-      <c r="C211">
-        <v>29.166666670000001</v>
-      </c>
-      <c r="D211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4">
-      <c r="A212" t="s">
-        <v>210</v>
-      </c>
-      <c r="B212">
-        <v>18.18181818</v>
-      </c>
-      <c r="C212">
-        <v>9.0909090910000003</v>
-      </c>
-      <c r="D212">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4">
-      <c r="A213" t="s">
-        <v>211</v>
-      </c>
-      <c r="B213">
-        <v>13.636363640000001</v>
-      </c>
-      <c r="C213">
-        <v>27.272727270000001</v>
-      </c>
-      <c r="D213">
-        <v>4.5454545450000001</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4">
-      <c r="A214" t="s">
-        <v>212</v>
-      </c>
-      <c r="B214">
-        <v>33.333333330000002</v>
-      </c>
-      <c r="C214">
-        <v>0</v>
-      </c>
-      <c r="D214">
-        <v>13.33333333</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4">
-      <c r="A215" t="s">
-        <v>213</v>
-      </c>
-      <c r="B215">
-        <v>33.333333330000002</v>
-      </c>
-      <c r="C215">
-        <v>20</v>
-      </c>
-      <c r="D215">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4">
-      <c r="A216" t="s">
-        <v>214</v>
-      </c>
-      <c r="B216">
-        <v>14.47368421</v>
-      </c>
-      <c r="C216">
-        <v>17.10526316</v>
-      </c>
-      <c r="D216">
-        <v>2.6315789469999999</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4">
-      <c r="A217" t="s">
-        <v>215</v>
-      </c>
-      <c r="B217">
-        <v>6.896551724</v>
-      </c>
-      <c r="C217">
-        <v>15.51724138</v>
-      </c>
-      <c r="D217">
-        <v>1.724137931</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4">
-      <c r="A218" t="s">
-        <v>216</v>
-      </c>
-      <c r="B218">
-        <v>14.81481481</v>
-      </c>
-      <c r="C218">
-        <v>22.222222219999999</v>
-      </c>
-      <c r="D218">
-        <v>11.11111111</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4">
-      <c r="A219" t="s">
-        <v>217</v>
-      </c>
-      <c r="B219">
-        <v>8.1632653059999996</v>
-      </c>
-      <c r="C219">
-        <v>29.591836730000001</v>
-      </c>
-      <c r="D219">
-        <v>6.1224489799999997</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4">
-      <c r="A220" t="s">
-        <v>218</v>
-      </c>
-      <c r="B220">
-        <v>27.777777780000001</v>
-      </c>
-      <c r="C220">
-        <v>33.333333330000002</v>
-      </c>
-      <c r="D220">
-        <v>5.5555555559999998</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4">
-      <c r="A221" t="s">
-        <v>219</v>
-      </c>
-      <c r="B221">
-        <v>18.18181818</v>
-      </c>
-      <c r="C221">
-        <v>50</v>
-      </c>
-      <c r="D221">
-        <v>4.5454545450000001</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4">
-      <c r="A222" t="s">
-        <v>220</v>
-      </c>
-      <c r="B222">
-        <v>16</v>
-      </c>
-      <c r="C222">
-        <v>48</v>
-      </c>
-      <c r="D222">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4">
-      <c r="A223" t="s">
-        <v>221</v>
-      </c>
-      <c r="B223">
-        <v>18.18181818</v>
-      </c>
-      <c r="C223">
-        <v>40.909090910000003</v>
-      </c>
-      <c r="D223">
-        <v>4.5454545450000001</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4">
-      <c r="A224" t="s">
-        <v>222</v>
-      </c>
-      <c r="B224">
-        <v>20</v>
-      </c>
-      <c r="C224">
-        <v>56</v>
-      </c>
-      <c r="D224">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4">
-      <c r="A225" t="s">
-        <v>223</v>
-      </c>
-      <c r="B225">
-        <v>31.25</v>
-      </c>
-      <c r="C225">
-        <v>10.41666667</v>
-      </c>
-      <c r="D225">
-        <v>4.1666666670000003</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4">
-      <c r="A226" t="s">
-        <v>224</v>
-      </c>
-      <c r="B226">
-        <v>28.571428569999998</v>
-      </c>
-      <c r="C226">
-        <v>25</v>
-      </c>
-      <c r="D226">
-        <v>7.1428571429999996</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4">
-      <c r="A227" t="s">
-        <v>225</v>
-      </c>
-      <c r="B227">
-        <v>32.558139529999998</v>
-      </c>
-      <c r="C227">
-        <v>13.953488370000001</v>
-      </c>
-      <c r="D227">
-        <v>9.3023255809999998</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4">
-      <c r="A228" t="s">
-        <v>226</v>
-      </c>
-      <c r="B228">
-        <v>28</v>
-      </c>
-      <c r="C228">
-        <v>28</v>
-      </c>
-      <c r="D228">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4">
-      <c r="A229" t="s">
-        <v>227</v>
-      </c>
-      <c r="B229">
-        <v>24.390243900000002</v>
-      </c>
-      <c r="C229">
-        <v>24.390243900000002</v>
-      </c>
-      <c r="D229">
-        <v>4.8780487800000003</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4">
-      <c r="A230" t="s">
-        <v>228</v>
-      </c>
-      <c r="B230">
-        <v>26</v>
-      </c>
-      <c r="C230">
-        <v>24</v>
-      </c>
-      <c r="D230">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4">
-      <c r="A231" t="s">
-        <v>229</v>
-      </c>
-      <c r="B231">
-        <v>15.78947368</v>
-      </c>
-      <c r="C231">
-        <v>28.94736842</v>
-      </c>
-      <c r="D231">
-        <v>5.263157895</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4">
-      <c r="A232" t="s">
-        <v>230</v>
-      </c>
-      <c r="B232">
-        <v>16.129032259999999</v>
-      </c>
-      <c r="C232">
-        <v>9.6774193549999996</v>
-      </c>
-      <c r="D232">
-        <v>9.6774193549999996</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4">
-      <c r="A233" t="s">
-        <v>231</v>
-      </c>
-      <c r="B233">
-        <v>9.6774193549999996</v>
-      </c>
-      <c r="C233">
-        <v>38.709677419999998</v>
-      </c>
-      <c r="D233">
-        <v>19.354838709999999</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4">
-      <c r="A234" t="s">
-        <v>232</v>
-      </c>
-      <c r="B234">
-        <v>22.44897959</v>
-      </c>
-      <c r="C234">
-        <v>26.53061224</v>
-      </c>
-      <c r="D234">
-        <v>8.1632653059999996</v>
+        <v>0.494503582</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D234">
+  <conditionalFormatting sqref="B2:B208">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF6600"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C208">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D208">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color theme="0"/>
-        <color rgb="FFFF0000"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>